<commit_message>
Reload data data erasing solved
</commit_message>
<xml_diff>
--- a/Files/GreenInputData.xlsx
+++ b/Files/GreenInputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neelpatel/Drive/JAY Assignment/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windsor - Master\3rd Semester\SoftwareProject\third feb\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D69336-05AB-BB45-898A-307A5481960E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF18B878-8E85-4FCA-BFE4-231136AFAA94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17300" xr2:uid="{65B25BE0-00A2-AF45-AABE-1253AC379FF7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{65B25BE0-00A2-AF45-AABE-1253AC379FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -84,6 +73,27 @@
   </si>
   <si>
     <t>G30</t>
+  </si>
+  <si>
+    <t>Des2</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Des 3</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Q2</t>
   </si>
 </sst>
 </file>
@@ -458,21 +468,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F8AC1A-671B-CF48-A92B-0C5E8445FCD2}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.69921875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="12.69921875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,7 +514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -534,6 +544,70 @@
       </c>
       <c r="J2" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1">
+        <v>982514</v>
+      </c>
+      <c r="G3" s="1">
+        <v>258</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1">
+        <v>98512</v>
+      </c>
+      <c r="G4" s="1">
+        <v>258</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>